<commit_message>
workflow and db created
</commit_message>
<xml_diff>
--- a/workflow_screens.xlsx
+++ b/workflow_screens.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\helpfulresources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292FD77-42D1-48EF-ACD2-A4E7A1478E7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF97D1EA-8676-4A34-A627-5E622F024EF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8615CF93-DBA5-4DB8-B415-73D5AAACBE0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8615CF93-DBA5-4DB8-B415-73D5AAACBE0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>User type</t>
   </si>
@@ -56,6 +57,75 @@
   </si>
   <si>
     <t xml:space="preserve">will have access to edit articles + edit prayer </t>
+  </si>
+  <si>
+    <t>table Name:</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>sample value</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Table name:</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>article title</t>
+  </si>
+  <si>
+    <t>article body</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>published datetime</t>
+  </si>
+  <si>
+    <t>article description</t>
+  </si>
+  <si>
+    <t>prayers</t>
+  </si>
+  <si>
+    <t>prayer cell name</t>
+  </si>
+  <si>
+    <t>cell leader</t>
+  </si>
+  <si>
+    <t>cell members</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>prayer logs</t>
+  </si>
+  <si>
+    <t>prayercellid</t>
+  </si>
+  <si>
+    <t>thank God for</t>
+  </si>
+  <si>
+    <t>Pray for</t>
+  </si>
+  <si>
+    <t>entrydatetime</t>
+  </si>
+  <si>
+    <t>articles</t>
   </si>
 </sst>
 </file>
@@ -798,25 +868,78 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8832C08-0648-4108-87E7-B2CF03345B10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4981575" y="5553075"/>
+          <a:ext cx="1162050" cy="1933575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>287111</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>164645</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>480332</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>155120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9200D161-D34C-4FAF-B14D-261BCE72B05B}"/>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70E177EA-DBE3-4677-9519-973633E412CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -839,8 +962,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5629275" y="7429500"/>
-          <a:ext cx="2800350" cy="2428875"/>
+          <a:off x="3348718" y="11975645"/>
+          <a:ext cx="3867150" cy="1704975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -861,23 +984,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8832C08-0648-4108-87E7-B2CF03345B10}"/>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11011CC3-B289-4E9C-A87F-6FFC5B545145}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -885,8 +1008,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4981575" y="5553075"/>
-          <a:ext cx="1162050" cy="1933575"/>
+          <a:off x="666750" y="1581150"/>
+          <a:ext cx="3657600" cy="10306050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -910,6 +1033,751 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>165652</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>588065</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFE701D2-DA92-4F99-9B14-487EB44DF71E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4456043" y="9674087"/>
+          <a:ext cx="4712805" cy="2716696"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323022</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>99392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>380172</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>185117</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A07FAFCF-4CA1-4886-8BC7-0FC5E02C5366}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1548848" y="14958392"/>
+          <a:ext cx="3734628" cy="2562225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1E4B0D1-289D-440B-9B08-3FEE01D6DBE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="571500" y="1651000"/>
+          <a:ext cx="2190750" cy="13303250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{466A0FCB-3636-47B1-8EA3-4EB111E47AF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9201150" y="8991600"/>
+          <a:ext cx="2552700" cy="4524375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2283F7A3-4D8C-441A-8995-372BF59E1C01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3276600" y="18430875"/>
+          <a:ext cx="1971675" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA1DE79E-14F8-4B49-814B-826430279477}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3038475" y="17345025"/>
+          <a:ext cx="800100" cy="1190625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C628DA4D-AAB7-4DBF-ADEF-D36E28FBC9A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11915775" y="16563975"/>
+          <a:ext cx="1876425" cy="1771650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B8DBB6-6E0C-4004-9C59-38E19687D76D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2533650" y="14601825"/>
+          <a:ext cx="4933950" cy="1057275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Arrow Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47DD9581-942A-4B22-A1BC-E2A0DCA8CD41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11191875" y="14497050"/>
+          <a:ext cx="933450" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>70757</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6BD59C6-E810-4657-A7C9-601DC742461B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6844393" y="14491607"/>
+          <a:ext cx="4438650" cy="5772150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9B16DF2-7F8C-4D54-846A-841F39216574}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10164536" y="16754475"/>
+          <a:ext cx="2050596" cy="2281918"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>214992</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35871103-13F0-4902-A2EA-BC1FD85C36A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12328071" y="14151429"/>
+          <a:ext cx="1970314" cy="2381250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>312965</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>551090</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>110218</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C33D9F4-E44B-4700-878D-BA9E07332671}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5211536" y="7511143"/>
+          <a:ext cx="2687411" cy="2886075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1214,23 +2082,170 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBD4F62-77D5-454E-B573-EDACDD554333}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U48" sqref="U48"/>
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y41" sqref="Y41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FA81465-0B88-49D7-BC46-D96156AA9649}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB3BA1E-F3EA-4895-8F24-8728262C9D68}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>